<commit_message>
py working with excel
</commit_message>
<xml_diff>
--- a/excels/РЕЙТИНГ с изм.2.xlsx
+++ b/excels/РЕЙТИНГ с изм.2.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="278">
   <si>
     <t xml:space="preserve">Перечень</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve"> за 2021 год</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kolledge1</t>
   </si>
   <si>
     <t xml:space="preserve">N п/п</t>
@@ -2036,10 +2039,10 @@
   <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E155" activeCellId="0" sqref="E155"/>
+      <selection pane="topLeft" activeCell="E143" activeCellId="0" sqref="E143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="35.42"/>
@@ -2048,7 +2051,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="43.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="2" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2084,8 +2087,10 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
+    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -2095,30 +2100,30 @@
     </row>
     <row r="5" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -2129,16 +2134,16 @@
     </row>
     <row r="7" customFormat="false" ht="77.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="15" t="n">
         <v>3</v>
@@ -2147,7 +2152,7 @@
         <v>100</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2155,16 +2160,16 @@
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2172,37 +2177,37 @@
       <c r="B9" s="13"/>
       <c r="C9" s="14"/>
       <c r="D9" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2210,12 +2215,12 @@
       <c r="B11" s="23"/>
       <c r="C11" s="13"/>
       <c r="D11" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="24"/>
       <c r="G11" s="27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2223,7 +2228,7 @@
       <c r="B12" s="23"/>
       <c r="C12" s="13"/>
       <c r="D12" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="10" t="n">
         <v>1</v>
@@ -2237,19 +2242,19 @@
       <c r="A13" s="14"/>
       <c r="B13" s="23"/>
       <c r="C13" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" s="30" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2257,12 +2262,12 @@
       <c r="B14" s="23"/>
       <c r="C14" s="14"/>
       <c r="D14" s="29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="14"/>
       <c r="G14" s="32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,7 +2275,7 @@
       <c r="B15" s="23"/>
       <c r="C15" s="14"/>
       <c r="D15" s="21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="14"/>
@@ -2278,25 +2283,25 @@
     </row>
     <row r="16" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E16" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,19 +2321,19 @@
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="30" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2336,12 +2341,12 @@
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="14"/>
       <c r="G19" s="20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2349,7 +2354,7 @@
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="14"/>
@@ -2363,30 +2368,30 @@
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" s="36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F23" s="36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="37" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="37"/>
@@ -2394,30 +2399,30 @@
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="38" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" s="15" t="n">
         <v>3</v>
       </c>
       <c r="F25" s="39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G25" s="40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2425,12 +2430,12 @@
       <c r="B26" s="30"/>
       <c r="C26" s="14"/>
       <c r="D26" s="29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="39"/>
       <c r="G26" s="41" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,7 +2443,7 @@
       <c r="B27" s="30"/>
       <c r="C27" s="14"/>
       <c r="D27" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="39"/>
@@ -2449,13 +2454,13 @@
       <c r="B28" s="30"/>
       <c r="C28" s="14"/>
       <c r="D28" s="42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E28" s="43" t="n">
         <v>2</v>
       </c>
       <c r="F28" s="44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G28" s="41"/>
     </row>
@@ -2468,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G29" s="41"/>
     </row>
@@ -2476,19 +2481,19 @@
       <c r="A30" s="30"/>
       <c r="B30" s="30"/>
       <c r="C30" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E30" s="15" t="n">
         <v>3</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G30" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,16 +2501,16 @@
       <c r="B31" s="30"/>
       <c r="C31" s="14"/>
       <c r="D31" s="29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E31" s="18" t="n">
         <v>2</v>
       </c>
       <c r="F31" s="46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2513,13 +2518,13 @@
       <c r="B32" s="30"/>
       <c r="C32" s="14"/>
       <c r="D32" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E32" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G32" s="9"/>
     </row>
@@ -2527,19 +2532,19 @@
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E33" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F33" s="39" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G33" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2547,12 +2552,12 @@
       <c r="B34" s="30"/>
       <c r="C34" s="14"/>
       <c r="D34" s="29" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="39"/>
       <c r="G34" s="49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2560,37 +2565,37 @@
       <c r="B35" s="30"/>
       <c r="C35" s="14"/>
       <c r="D35" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E35" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E36" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G36" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,29 +2616,29 @@
         <v>1</v>
       </c>
       <c r="F38" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G38" s="50"/>
     </row>
     <row r="39" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14"/>
       <c r="B39" s="23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E39" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F39" s="53" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G39" s="54" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,31 +2650,31 @@
         <v>1</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G40" s="54"/>
     </row>
     <row r="41" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E41" s="15" t="n">
         <v>4</v>
       </c>
       <c r="F41" s="53" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G41" s="54" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2681,29 +2686,29 @@
         <v>2</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G42" s="54"/>
     </row>
     <row r="43" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="14"/>
       <c r="B43" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E43" s="15" t="n">
         <v>5</v>
       </c>
       <c r="F43" s="53" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G43" s="50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,7 +2720,7 @@
         <v>4</v>
       </c>
       <c r="F44" s="46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G44" s="50"/>
     </row>
@@ -2736,30 +2741,30 @@
     <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D48" s="36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E48" s="36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F48" s="36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G48" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B49" s="37"/>
       <c r="C49" s="37"/>
@@ -2770,25 +2775,25 @@
     </row>
     <row r="50" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D50" s="55" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E50" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F50" s="56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G50" s="50" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2809,16 +2814,16 @@
       <c r="B52" s="13"/>
       <c r="C52" s="55"/>
       <c r="D52" s="23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E52" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F52" s="56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G52" s="50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2836,25 +2841,25 @@
     </row>
     <row r="54" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E54" s="30" t="n">
         <v>1</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G54" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,12 +2867,12 @@
       <c r="B55" s="23"/>
       <c r="C55" s="14"/>
       <c r="D55" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E55" s="30"/>
       <c r="F55" s="14"/>
       <c r="G55" s="49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2875,7 +2880,7 @@
       <c r="B56" s="23"/>
       <c r="C56" s="14"/>
       <c r="D56" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E56" s="30"/>
       <c r="F56" s="14"/>
@@ -2885,19 +2890,19 @@
       <c r="A57" s="14"/>
       <c r="B57" s="23"/>
       <c r="C57" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E57" s="58" t="n">
         <v>1</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G57" s="49" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,12 +2910,12 @@
       <c r="B58" s="23"/>
       <c r="C58" s="9"/>
       <c r="D58" s="29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E58" s="58"/>
       <c r="F58" s="9"/>
       <c r="G58" s="49" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,7 +2923,7 @@
       <c r="B59" s="23"/>
       <c r="C59" s="9"/>
       <c r="D59" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E59" s="58"/>
       <c r="F59" s="9"/>
@@ -2926,25 +2931,25 @@
     </row>
     <row r="60" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E60" s="15" t="n">
         <v>1</v>
       </c>
       <c r="F60" s="39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G60" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2952,12 +2957,12 @@
       <c r="B61" s="23"/>
       <c r="C61" s="14"/>
       <c r="D61" s="29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="39"/>
       <c r="G61" s="59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,37 +2970,37 @@
       <c r="B62" s="23"/>
       <c r="C62" s="14"/>
       <c r="D62" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E62" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="F62" s="28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G62" s="32"/>
     </row>
     <row r="63" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C63" s="60" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D63" s="61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E63" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F63" s="33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G63" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3003,16 +3008,16 @@
       <c r="B64" s="23"/>
       <c r="C64" s="60"/>
       <c r="D64" s="61" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E64" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F64" s="44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G64" s="49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,7 +3025,7 @@
       <c r="B65" s="23"/>
       <c r="C65" s="60"/>
       <c r="D65" s="61" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E65" s="51"/>
       <c r="F65" s="52"/>
@@ -3028,16 +3033,16 @@
     </row>
     <row r="66" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="14" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D66" s="62" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E66" s="15" t="n">
         <v>3</v>
@@ -3046,15 +3051,15 @@
         <v>100</v>
       </c>
       <c r="G66" s="23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="14"/>
       <c r="B67" s="23"/>
       <c r="C67" s="23"/>
-      <c r="D67" s="26" t="s">
-        <v>137</v>
+      <c r="D67" s="32" t="s">
+        <v>138</v>
       </c>
       <c r="E67" s="15"/>
       <c r="F67" s="24"/>
@@ -3069,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="F68" s="57" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G68" s="23"/>
     </row>
@@ -3078,37 +3083,37 @@
       <c r="B69" s="23"/>
       <c r="C69" s="23"/>
       <c r="D69" s="63" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E69" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F69" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G69" s="23"/>
     </row>
     <row r="70" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B70" s="63" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C70" s="63" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E70" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F70" s="63" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G70" s="64" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,30 +3138,30 @@
     </row>
     <row r="73" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" s="36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E73" s="36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F73" s="36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G73" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="11"/>
@@ -3167,16 +3172,16 @@
     </row>
     <row r="75" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E75" s="30" t="n">
         <v>5</v>
@@ -3185,7 +3190,7 @@
         <v>0.95</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3193,12 +3198,12 @@
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
       <c r="D76" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E76" s="30"/>
       <c r="F76" s="69"/>
       <c r="G76" s="49" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="71.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3206,31 +3211,31 @@
       <c r="B77" s="14"/>
       <c r="C77" s="14"/>
       <c r="D77" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E77" s="30"/>
       <c r="F77" s="69"/>
       <c r="G77" s="70" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="14"/>
       <c r="B78" s="14"/>
       <c r="C78" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E78" s="30" t="n">
         <v>5</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3238,7 +3243,7 @@
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="29" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E79" s="30"/>
       <c r="F79" s="14"/>
@@ -3249,7 +3254,7 @@
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
       <c r="D80" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E80" s="30"/>
       <c r="F80" s="14"/>
@@ -3259,19 +3264,19 @@
       <c r="A81" s="14"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E81" s="15" t="n">
         <v>5</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G81" s="31" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3279,16 +3284,16 @@
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
       <c r="D82" s="29" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E82" s="43" t="n">
         <v>4</v>
       </c>
       <c r="F82" s="71" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G82" s="20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3296,13 +3301,13 @@
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
       <c r="D83" s="29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E83" s="43" t="n">
         <v>3</v>
       </c>
       <c r="F83" s="71" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G83" s="20"/>
     </row>
@@ -3315,7 +3320,7 @@
         <v>2</v>
       </c>
       <c r="F84" s="71" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G84" s="20"/>
     </row>
@@ -3328,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="72" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G85" s="20"/>
     </row>
@@ -3354,30 +3359,30 @@
     </row>
     <row r="88" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B88" s="36" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C88" s="36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D88" s="36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E88" s="36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F88" s="36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G88" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
@@ -3388,25 +3393,25 @@
     </row>
     <row r="90" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="14" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D90" s="73" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E90" s="15" t="n">
         <v>3</v>
       </c>
       <c r="F90" s="53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G90" s="35" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,16 +3419,16 @@
       <c r="B91" s="14"/>
       <c r="C91" s="23"/>
       <c r="D91" s="73" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E91" s="43" t="n">
         <v>2</v>
       </c>
       <c r="F91" s="74" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G91" s="75" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,16 +3436,16 @@
       <c r="B92" s="14"/>
       <c r="C92" s="23"/>
       <c r="D92" s="73" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E92" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F92" s="74" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G92" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3448,13 +3453,13 @@
       <c r="B93" s="14"/>
       <c r="C93" s="23"/>
       <c r="D93" s="22" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E93" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="F93" s="34" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G93" s="9"/>
     </row>
@@ -3462,19 +3467,19 @@
       <c r="A94" s="14"/>
       <c r="B94" s="14"/>
       <c r="C94" s="23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D94" s="73" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E94" s="15" t="n">
         <v>3</v>
       </c>
       <c r="F94" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G94" s="35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3482,16 +3487,16 @@
       <c r="B95" s="14"/>
       <c r="C95" s="23"/>
       <c r="D95" s="76" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E95" s="43" t="n">
         <v>2</v>
       </c>
       <c r="F95" s="74" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G95" s="49" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3499,13 +3504,13 @@
       <c r="B96" s="14"/>
       <c r="C96" s="23"/>
       <c r="D96" s="76" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E96" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F96" s="74" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G96" s="17"/>
     </row>
@@ -3518,7 +3523,7 @@
         <v>0.5</v>
       </c>
       <c r="F97" s="34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G97" s="9"/>
     </row>
@@ -3526,19 +3531,19 @@
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="23" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D98" s="77" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E98" s="78" t="n">
         <v>3</v>
       </c>
       <c r="F98" s="79" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G98" s="31" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,16 +3551,16 @@
       <c r="B99" s="14"/>
       <c r="C99" s="23"/>
       <c r="D99" s="80" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E99" s="51" t="n">
         <v>2</v>
       </c>
       <c r="F99" s="81" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G99" s="17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3567,7 +3572,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="81" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G100" s="17"/>
     </row>
@@ -3576,13 +3581,13 @@
       <c r="B101" s="14"/>
       <c r="C101" s="23"/>
       <c r="D101" s="8" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E101" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="F101" s="34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G101" s="9"/>
     </row>
@@ -3590,19 +3595,19 @@
       <c r="A102" s="14"/>
       <c r="B102" s="14"/>
       <c r="C102" s="32" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D102" s="29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E102" s="58" t="n">
         <v>1</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G102" s="49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,12 +3615,12 @@
       <c r="B103" s="14"/>
       <c r="C103" s="32"/>
       <c r="D103" s="29" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E103" s="58"/>
       <c r="F103" s="9"/>
       <c r="G103" s="49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3623,7 +3628,7 @@
       <c r="B104" s="14"/>
       <c r="C104" s="32"/>
       <c r="D104" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E104" s="58"/>
       <c r="F104" s="9"/>
@@ -3631,25 +3636,25 @@
     </row>
     <row r="105" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="30" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D105" s="29" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E105" s="15" t="n">
         <v>3</v>
       </c>
       <c r="F105" s="82" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G105" s="35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3657,12 +3662,12 @@
       <c r="B106" s="23"/>
       <c r="C106" s="14"/>
       <c r="D106" s="29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E106" s="15"/>
       <c r="F106" s="82"/>
       <c r="G106" s="49" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,7 +3675,7 @@
       <c r="B107" s="23"/>
       <c r="C107" s="14"/>
       <c r="D107" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E107" s="15"/>
       <c r="F107" s="82"/>
@@ -3706,19 +3711,19 @@
       <c r="A110" s="30"/>
       <c r="B110" s="23"/>
       <c r="C110" s="23" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D110" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E110" s="78" t="n">
         <v>2</v>
       </c>
       <c r="F110" s="83" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G110" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,7 +3731,7 @@
       <c r="B111" s="23"/>
       <c r="C111" s="23"/>
       <c r="D111" s="29" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E111" s="51" t="n">
         <v>1</v>
@@ -3735,7 +3740,7 @@
         <v>0.2</v>
       </c>
       <c r="G111" s="49" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,7 +3748,7 @@
       <c r="B112" s="23"/>
       <c r="C112" s="23"/>
       <c r="D112" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E112" s="10"/>
       <c r="F112" s="28"/>
@@ -3753,10 +3758,10 @@
       <c r="A113" s="30"/>
       <c r="B113" s="23"/>
       <c r="C113" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D113" s="48" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E113" s="78" t="n">
         <v>1</v>
@@ -3765,7 +3770,7 @@
         <v>100</v>
       </c>
       <c r="G113" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3773,12 +3778,12 @@
       <c r="B114" s="23"/>
       <c r="C114" s="23"/>
       <c r="D114" s="29" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E114" s="51"/>
       <c r="F114" s="84"/>
       <c r="G114" s="49" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,7 +3791,7 @@
       <c r="B115" s="23"/>
       <c r="C115" s="23"/>
       <c r="D115" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E115" s="10"/>
       <c r="F115" s="28"/>
@@ -3795,11 +3800,11 @@
     <row r="116" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="30"/>
       <c r="B116" s="23"/>
-      <c r="C116" s="55" t="s">
-        <v>218</v>
+      <c r="C116" s="23" t="s">
+        <v>219</v>
       </c>
       <c r="D116" s="48" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E116" s="51" t="n">
         <v>1</v>
@@ -3808,7 +3813,7 @@
         <v>100</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3816,12 +3821,12 @@
       <c r="B117" s="23"/>
       <c r="C117" s="23"/>
       <c r="D117" s="29" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E117" s="51"/>
       <c r="F117" s="84"/>
       <c r="G117" s="49" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3829,7 +3834,7 @@
       <c r="B118" s="23"/>
       <c r="C118" s="23"/>
       <c r="D118" s="29" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E118" s="51"/>
       <c r="F118" s="84"/>
@@ -3839,19 +3844,19 @@
       <c r="A119" s="30"/>
       <c r="B119" s="23"/>
       <c r="C119" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D119" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E119" s="78" t="n">
         <v>2</v>
       </c>
       <c r="F119" s="83" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G119" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,7 +3864,7 @@
       <c r="B120" s="23"/>
       <c r="C120" s="23"/>
       <c r="D120" s="29" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E120" s="51" t="n">
         <v>1</v>
@@ -3868,7 +3873,7 @@
         <v>5</v>
       </c>
       <c r="G120" s="31" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3876,7 +3881,7 @@
       <c r="B121" s="23"/>
       <c r="C121" s="23"/>
       <c r="D121" s="21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E121" s="10"/>
       <c r="F121" s="28"/>
@@ -3884,25 +3889,25 @@
     </row>
     <row r="122" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="30" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B122" s="23" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C122" s="55" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D122" s="48" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E122" s="78" t="n">
         <v>1</v>
       </c>
       <c r="F122" s="83" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G122" s="31" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3927,19 +3932,19 @@
       <c r="A125" s="30"/>
       <c r="B125" s="23"/>
       <c r="C125" s="55" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D125" s="48" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E125" s="78" t="n">
         <v>1</v>
       </c>
       <c r="F125" s="83" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G125" s="31" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,19 +3969,19 @@
       <c r="A128" s="30"/>
       <c r="B128" s="23"/>
       <c r="C128" s="55" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D128" s="48" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E128" s="78" t="n">
         <v>1</v>
       </c>
       <c r="F128" s="83" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G128" s="31" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3999,25 +4004,25 @@
     </row>
     <row r="131" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B131" s="76" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C131" s="85" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E131" s="86" t="n">
         <v>1</v>
       </c>
       <c r="F131" s="55" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G131" s="50" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4025,7 +4030,7 @@
       <c r="B132" s="76"/>
       <c r="C132" s="85"/>
       <c r="D132" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E132" s="86"/>
       <c r="F132" s="55"/>
@@ -4036,7 +4041,7 @@
       <c r="B133" s="76"/>
       <c r="C133" s="85"/>
       <c r="D133" s="17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E133" s="86"/>
       <c r="F133" s="55"/>
@@ -4044,16 +4049,16 @@
     </row>
     <row r="134" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="30" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B134" s="87" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D134" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E134" s="88" t="n">
         <v>1</v>
@@ -4062,7 +4067,7 @@
         <v>100</v>
       </c>
       <c r="G134" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4070,12 +4075,12 @@
       <c r="B135" s="87"/>
       <c r="C135" s="23"/>
       <c r="D135" s="17" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E135" s="86"/>
       <c r="F135" s="26"/>
       <c r="G135" s="31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4083,7 +4088,7 @@
       <c r="B136" s="87"/>
       <c r="C136" s="23"/>
       <c r="D136" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E136" s="89"/>
       <c r="F136" s="32"/>
@@ -4111,7 +4116,7 @@
     </row>
     <row r="139" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="37" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B139" s="37"/>
       <c r="C139" s="37"/>
@@ -4122,25 +4127,25 @@
     </row>
     <row r="140" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C140" s="14" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D140" s="48" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E140" s="15" t="n">
         <v>3</v>
       </c>
       <c r="F140" s="53" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G140" s="92" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4148,16 +4153,16 @@
       <c r="B141" s="23"/>
       <c r="C141" s="14"/>
       <c r="D141" s="29" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E141" s="43" t="n">
         <v>2</v>
       </c>
       <c r="F141" s="44" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G141" s="93" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4165,13 +4170,13 @@
       <c r="B142" s="23"/>
       <c r="C142" s="14"/>
       <c r="D142" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E142" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F142" s="28" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G142" s="93"/>
     </row>
@@ -4180,7 +4185,9 @@
       <c r="B143" s="66"/>
       <c r="C143" s="66"/>
       <c r="D143" s="66"/>
-      <c r="E143" s="67"/>
+      <c r="E143" s="67" t="n">
+        <v>7</v>
+      </c>
       <c r="F143" s="68"/>
       <c r="G143" s="66"/>
     </row>
@@ -4195,7 +4202,7 @@
     </row>
     <row r="145" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="37" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B145" s="37"/>
       <c r="C145" s="37"/>
@@ -4206,25 +4213,25 @@
     </row>
     <row r="146" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="30" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D146" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E146" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F146" s="53" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G146" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4232,16 +4239,16 @@
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
       <c r="D147" s="29" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E147" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F147" s="74" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G147" s="94" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,37 +4256,37 @@
       <c r="B148" s="14"/>
       <c r="C148" s="14"/>
       <c r="D148" s="21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E148" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="F148" s="34" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G148" s="94"/>
     </row>
     <row r="149" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="30" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B149" s="14" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D149" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E149" s="15" t="n">
         <v>2</v>
       </c>
       <c r="F149" s="53" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G149" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4287,16 +4294,16 @@
       <c r="B150" s="14"/>
       <c r="C150" s="14"/>
       <c r="D150" s="29" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E150" s="43" t="n">
         <v>1</v>
       </c>
       <c r="F150" s="95" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G150" s="94" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4304,13 +4311,13 @@
       <c r="B151" s="14"/>
       <c r="C151" s="14"/>
       <c r="D151" s="21" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E151" s="10" t="n">
         <v>0.5</v>
       </c>
       <c r="F151" s="34" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G151" s="94"/>
     </row>
@@ -4321,10 +4328,10 @@
     </row>
     <row r="153" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D153" s="96" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E153" s="97" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F153" s="98" t="n">
         <v>1</v>

</xml_diff>